<commit_message>
all the datasets updated still minor fixes required
</commit_message>
<xml_diff>
--- a/frontend/public/Data/workshops/2023-2024.xlsx
+++ b/frontend/public/Data/workshops/2023-2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaushik\OneDrive\Desktop\cse dept latest\CSE\frontend\src\Data\workshops\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaushik\OneDrive\Desktop\cse dept latest\CSE\frontend\public\Data\workshops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736463B3-FD47-4C94-8713-8EEC2A82FBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044B03F2-AE61-4259-A790-7864AA5AD4F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D0EE93CC-E330-41C2-B128-14208B60EA23}"/>
   </bookViews>
@@ -208,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -234,6 +234,10 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,9 +574,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D025FDF2-E597-4EFC-862F-EF17D56661B1}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="12.5546875" style="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
@@ -584,7 +593,7 @@
       <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
@@ -607,7 +616,7 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -630,7 +639,7 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -653,7 +662,7 @@
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -676,7 +685,7 @@
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -695,7 +704,7 @@
       <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -704,7 +713,7 @@
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>

</xml_diff>